<commit_message>
made initial data transformation
</commit_message>
<xml_diff>
--- a/data/davie trainingsplan 2014.xlsx
+++ b/data/davie trainingsplan 2014.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\OneDrive\Documents\Evernote\145316853\external-edits\9f0a33e8-1105-57a6-e292-247fcab8acb4\59872577d82c18ce7f3dcbee5e22939d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\davie_trainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07589011-C61B-4F81-8B0E-A007712A2C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1851B3-47AC-49EC-A043-0D34FA76B716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-12615" windowWidth="38640" windowHeight="21120" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Planke set 1</t>
   </si>
@@ -56,24 +56,6 @@
     <t>Liegestütz set 3</t>
   </si>
   <si>
-    <t>Hammer Curls set 1</t>
-  </si>
-  <si>
-    <t>Hammer Curls set 2</t>
-  </si>
-  <si>
-    <t>Hammer Curls set 3</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 1</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 2</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 3</t>
-  </si>
-  <si>
     <t>Kniebeugen set 1</t>
   </si>
   <si>
@@ -83,57 +65,15 @@
     <t>Kniebeugen set 3</t>
   </si>
   <si>
-    <t>Turm Rudern set 1</t>
-  </si>
-  <si>
-    <t>Turm Rudern set 2</t>
-  </si>
-  <si>
-    <t>Turm Rudern set 3</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 1</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 2</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 3</t>
-  </si>
-  <si>
     <t>Planke set 4</t>
   </si>
   <si>
     <t>Liegestütz set 4</t>
   </si>
   <si>
-    <t>Hammer Curls set 4</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 4</t>
-  </si>
-  <si>
     <t>Kniebeugen set 4</t>
   </si>
   <si>
-    <t>Turm Rudern set 4</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 4</t>
-  </si>
-  <si>
-    <t>2, 12</t>
-  </si>
-  <si>
-    <t>2, 18</t>
-  </si>
-  <si>
-    <t>2, 15</t>
-  </si>
-  <si>
-    <t>2, 14</t>
-  </si>
-  <si>
     <t>20, 10</t>
   </si>
   <si>
@@ -146,10 +86,88 @@
     <t>20, 15</t>
   </si>
   <si>
-    <t>2, 10</t>
-  </si>
-  <si>
     <t>20, 19</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>2| 12</t>
+  </si>
+  <si>
+    <t>2 | 18</t>
+  </si>
+  <si>
+    <t>2 | 10</t>
+  </si>
+  <si>
+    <t>2 |15</t>
+  </si>
+  <si>
+    <t>2 | 14</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 1</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 2</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 3</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 4</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 1</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 2</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 3</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 4</t>
+  </si>
+  <si>
+    <t>Weighted Turm Rudern 
+set 4</t>
+  </si>
+  <si>
+    <t>Weighted 
+Turm Rudern 
+set 3</t>
+  </si>
+  <si>
+    <t>Weighted 
+Turm Rudern 
+set 2</t>
+  </si>
+  <si>
+    <t>Weighted 
+Turm Rudern 
+set 1</t>
+  </si>
+  <si>
+    <t>Weighted 
+Bizeps Curls 
+set 2</t>
+  </si>
+  <si>
+    <t>Weighted 
+Bizeps Curls 
+set 3</t>
+  </si>
+  <si>
+    <t>Weighted 
+Bizeps Curls 
+set 4</t>
+  </si>
+  <si>
+    <t>Weighted 
+Bizeps Curls 
+set 1</t>
   </si>
 </sst>
 </file>
@@ -206,12 +224,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -549,100 +570,102 @@
   <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="25" width="16.77734375" customWidth="1"/>
-    <col min="26" max="29" width="18.77734375" customWidth="1"/>
+    <col min="2" max="29" width="14.77734375" customWidth="1"/>
     <col min="30" max="46" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:29" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="S1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="T1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="U1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="V1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>27</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
@@ -662,10 +685,10 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="R2">
         <v>15</v>
@@ -674,10 +697,10 @@
         <v>15</v>
       </c>
       <c r="V2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="W2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -707,10 +730,10 @@
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="R5">
         <v>22</v>
@@ -719,10 +742,10 @@
         <v>15</v>
       </c>
       <c r="V5" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="W5" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
@@ -747,10 +770,10 @@
         <v>12</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="R7" s="3">
         <v>14</v>
@@ -759,13 +782,13 @@
         <v>25</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
implemented all the weights and current date in the plots
</commit_message>
<xml_diff>
--- a/data/davie trainingsplan 2014.xlsx
+++ b/data/davie trainingsplan 2014.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\davie_trainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFCC3A0-F356-4C44-9A68-4B8798A66B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18108726-7C50-4500-B16B-988EAE0BEDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Planke set 1</t>
   </si>
@@ -56,24 +56,6 @@
     <t>Liegestütz set 3</t>
   </si>
   <si>
-    <t>Hammer Curls set 1</t>
-  </si>
-  <si>
-    <t>Hammer Curls set 2</t>
-  </si>
-  <si>
-    <t>Hammer Curls set 3</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 1</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 2</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 3</t>
-  </si>
-  <si>
     <t>Kniebeugen set 1</t>
   </si>
   <si>
@@ -83,60 +65,15 @@
     <t>Kniebeugen set 3</t>
   </si>
   <si>
-    <t>Turm Rudern set 1</t>
-  </si>
-  <si>
-    <t>Turm Rudern set 2</t>
-  </si>
-  <si>
-    <t>Turm Rudern set 3</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 1</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 2</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 3</t>
-  </si>
-  <si>
     <t>Planke set 4</t>
   </si>
   <si>
     <t>Liegestütz set 4</t>
   </si>
   <si>
-    <t>Hammer Curls set 4</t>
-  </si>
-  <si>
-    <t>Bizeps Curls set 4</t>
-  </si>
-  <si>
     <t>Kniebeugen set 4</t>
   </si>
   <si>
-    <t>Turm Rudern set 4</t>
-  </si>
-  <si>
-    <t>Shoulder Press set 4</t>
-  </si>
-  <si>
-    <t>20, 10</t>
-  </si>
-  <si>
-    <t>20, 20</t>
-  </si>
-  <si>
-    <t>20, 12</t>
-  </si>
-  <si>
-    <t>20, 15</t>
-  </si>
-  <si>
-    <t>20, 19</t>
-  </si>
-  <si>
     <t>Datum</t>
   </si>
   <si>
@@ -158,25 +95,121 @@
     <t>2 | 9</t>
   </si>
   <si>
-    <t>20, 14</t>
-  </si>
-  <si>
     <t>2 | 15</t>
   </si>
   <si>
-    <t>30, 15</t>
-  </si>
-  <si>
-    <t>Turm Zug set 1</t>
-  </si>
-  <si>
-    <t>Turm Zug set 2</t>
-  </si>
-  <si>
-    <t>Turm Zug set 3</t>
-  </si>
-  <si>
-    <t>Turm Zug set 4</t>
+    <t>Waden set 1</t>
+  </si>
+  <si>
+    <t>Waden set 2</t>
+  </si>
+  <si>
+    <t>Waden set 3</t>
+  </si>
+  <si>
+    <t>Waden set 4</t>
+  </si>
+  <si>
+    <t>30 | 15</t>
+  </si>
+  <si>
+    <t>1 | 20 | 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 | 20 | 12</t>
+  </si>
+  <si>
+    <t>1 | 20 | 12</t>
+  </si>
+  <si>
+    <t>1 | 20 | 14</t>
+  </si>
+  <si>
+    <t>1 | 20 | 20</t>
+  </si>
+  <si>
+    <t>1 | 20 | 15</t>
+  </si>
+  <si>
+    <t>1 | 20 | 19</t>
+  </si>
+  <si>
+    <t>1,5 | 20 | 7</t>
+  </si>
+  <si>
+    <t>30 | 14</t>
+  </si>
+  <si>
+    <t>1,5 | 20 | 16</t>
+  </si>
+  <si>
+    <t>1,5 | 20 | 23</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 1</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 2</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 3</t>
+  </si>
+  <si>
+    <t>Weighted Hammer Curls set 4</t>
+  </si>
+  <si>
+    <t>Weighted Bizeps Curls set 1</t>
+  </si>
+  <si>
+    <t>Weighted Bizeps Curls set 2</t>
+  </si>
+  <si>
+    <t>Weighted Bizeps Curls set 3</t>
+  </si>
+  <si>
+    <t>Weighted Bizeps Curls set 4</t>
+  </si>
+  <si>
+    <t>Weighted Turm Rudern set 1</t>
+  </si>
+  <si>
+    <t>Weighted Turm Rudern set 2</t>
+  </si>
+  <si>
+    <t>Weighted Turm Rudern set 3</t>
+  </si>
+  <si>
+    <t>Weighted Turm Rudern set 4</t>
+  </si>
+  <si>
+    <t>Weighted Turm Zug set 1</t>
+  </si>
+  <si>
+    <t>Weighted Turm Zug set 2</t>
+  </si>
+  <si>
+    <t>Weighted Turm Zug set 3</t>
+  </si>
+  <si>
+    <t>Weighted Turm Zug set 4</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 1</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 2</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 3</t>
+  </si>
+  <si>
+    <t>Weighted Shoulder Press set 4</t>
+  </si>
+  <si>
+    <t>30 | 20</t>
+  </si>
+  <si>
+    <t>1,5 | 20 | 19</t>
   </si>
 </sst>
 </file>
@@ -227,13 +260,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -568,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6CF99-69E1-4DA6-A725-47BF4576CF35}">
-  <dimension ref="A1:AG16"/>
+  <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,108 +614,120 @@
     <col min="34" max="50" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:37" s="4" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="AK1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45515</v>
       </c>
@@ -698,10 +744,10 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="R2">
         <v>15</v>
@@ -710,23 +756,23 @@
         <v>15</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="W2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45516</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45517</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45518</v>
       </c>
@@ -743,10 +789,10 @@
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="R5">
         <v>22</v>
@@ -755,135 +801,298 @@
         <v>15</v>
       </c>
       <c r="V5" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" t="s">
         <v>30</v>
       </c>
-      <c r="W5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45519</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>45520</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>85</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7">
         <v>85</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7">
         <v>10</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <v>12</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="5">
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="5">
+      <c r="R7">
+        <v>14</v>
+      </c>
+      <c r="S7">
         <v>25</v>
       </c>
-      <c r="V7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="V7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W7" t="s">
+        <v>25</v>
+      </c>
+      <c r="X7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45521</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45522</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45523</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45524</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45525</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45526</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45527</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45528</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>45529</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>90</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>90</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>8</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16">
         <v>15</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" s="3">
+      <c r="J16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16">
         <v>15</v>
       </c>
-      <c r="S16" s="3">
+      <c r="S16">
         <v>12</v>
       </c>
-      <c r="V16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W16" s="3" t="s">
+      <c r="V16" t="s">
+        <v>28</v>
+      </c>
+      <c r="W16" t="s">
         <v>29</v>
       </c>
-      <c r="Z16" s="3" t="s">
-        <v>42</v>
+      <c r="Z16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45532</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45533</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45535</v>
+      </c>
+      <c r="B22">
+        <v>95</v>
+      </c>
+      <c r="C22">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>90</v>
+      </c>
+      <c r="F22">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" t="s">
+        <v>19</v>
+      </c>
+      <c r="R22">
+        <v>16</v>
+      </c>
+      <c r="S22">
+        <v>18</v>
+      </c>
+      <c r="V22" t="s">
+        <v>32</v>
+      </c>
+      <c r="W22" t="s">
+        <v>34</v>
+      </c>
+      <c r="X22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45538</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>45539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>45540</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>45541</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45542</v>
+      </c>
+      <c r="B29" s="3">
+        <v>100</v>
+      </c>
+      <c r="C29" s="3">
+        <v>95</v>
+      </c>
+      <c r="F29" s="3">
+        <v>11</v>
+      </c>
+      <c r="G29" s="3">
+        <v>19</v>
+      </c>
+      <c r="J29" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" t="s">
+        <v>17</v>
+      </c>
+      <c r="R29" s="3">
+        <v>20</v>
+      </c>
+      <c r="S29" s="3">
+        <v>24</v>
+      </c>
+      <c r="T29" s="3">
+        <v>20</v>
+      </c>
+      <c r="V29" t="s">
+        <v>34</v>
+      </c>
+      <c r="W29" t="s">
+        <v>57</v>
+      </c>
+      <c r="X29"/>
+      <c r="Z29" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH29">
+        <v>20</v>
+      </c>
+      <c r="AI29" s="3">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added calculations and  plots for avrg max and amount
</commit_message>
<xml_diff>
--- a/data/davie trainingsplan 2014.xlsx
+++ b/data/davie trainingsplan 2014.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\davie_trainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18108726-7C50-4500-B16B-988EAE0BEDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB478C9A-0176-4D80-9D73-D31B7D103C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
+    <workbookView xWindow="-38520" yWindow="-12615" windowWidth="38640" windowHeight="21120" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>Planke set 1</t>
   </si>
@@ -206,10 +206,28 @@
     <t>Weighted Shoulder Press set 4</t>
   </si>
   <si>
+    <t>1,5 | 20 | 19</t>
+  </si>
+  <si>
     <t>30 | 20</t>
   </si>
   <si>
-    <t>1,5 | 20 | 19</t>
+    <t>2 | 21</t>
+  </si>
+  <si>
+    <t>30 | 17</t>
+  </si>
+  <si>
+    <t>2 | 17</t>
+  </si>
+  <si>
+    <t>2 | 20 | 15</t>
+  </si>
+  <si>
+    <t>2 | 20 | 21</t>
+  </si>
+  <si>
+    <t>30 | 19</t>
   </si>
 </sst>
 </file>
@@ -602,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6CF99-69E1-4DA6-A725-47BF4576CF35}">
-  <dimension ref="A1:AK29"/>
+  <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,20 +1054,20 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>45542</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29">
         <v>100</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29">
         <v>95</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29">
         <v>11</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29">
         <v>19</v>
       </c>
       <c r="J29" t="s">
@@ -1061,24 +1079,23 @@
       <c r="L29" t="s">
         <v>17</v>
       </c>
-      <c r="R29" s="3">
+      <c r="R29">
         <v>20</v>
       </c>
-      <c r="S29" s="3">
+      <c r="S29">
         <v>24</v>
       </c>
-      <c r="T29" s="3">
+      <c r="T29">
         <v>20</v>
       </c>
       <c r="V29" t="s">
         <v>34</v>
       </c>
       <c r="W29" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z29" t="s">
         <v>57</v>
-      </c>
-      <c r="X29"/>
-      <c r="Z29" t="s">
-        <v>56</v>
       </c>
       <c r="AA29" t="s">
         <v>24</v>
@@ -1086,13 +1103,144 @@
       <c r="AH29">
         <v>20</v>
       </c>
-      <c r="AI29" s="3">
+      <c r="AI29">
         <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>45543</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>45544</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>45545</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>45546</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>45547</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>45548</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>45549</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>45550</v>
+      </c>
+      <c r="B37" s="3">
+        <v>100</v>
+      </c>
+      <c r="C37" s="3">
+        <v>100</v>
+      </c>
+      <c r="F37" s="3">
+        <v>24</v>
+      </c>
+      <c r="G37" s="3">
+        <v>24</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R37" s="3">
+        <v>30</v>
+      </c>
+      <c r="S37" s="3">
+        <v>25</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH37" s="3">
+        <v>20</v>
+      </c>
+      <c r="AI37" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>45551</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>45552</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>45554</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>45555</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>45556</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>45557</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>45558</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>45559</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>45560</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adjusted label sizes and format
</commit_message>
<xml_diff>
--- a/data/davie trainingsplan 2014.xlsx
+++ b/data/davie trainingsplan 2014.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\davie_trainer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvolf\python_projects\devie_trainer\davie_trainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB478C9A-0176-4D80-9D73-D31B7D103C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A756D4-7DBC-4EDA-9676-2AAC8EE1096F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-12615" windowWidth="38640" windowHeight="21120" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
+    <workbookView xWindow="-38520" yWindow="-10365" windowWidth="38640" windowHeight="21120" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -212,22 +212,22 @@
     <t>30 | 20</t>
   </si>
   <si>
+    <t>30 | 17</t>
+  </si>
+  <si>
+    <t>2 | 17</t>
+  </si>
+  <si>
+    <t>2 | 20 | 15</t>
+  </si>
+  <si>
+    <t>2 | 20 | 21</t>
+  </si>
+  <si>
+    <t>30 | 19</t>
+  </si>
+  <si>
     <t>2 | 21</t>
-  </si>
-  <si>
-    <t>30 | 17</t>
-  </si>
-  <si>
-    <t>2 | 17</t>
-  </si>
-  <si>
-    <t>2 | 20 | 15</t>
-  </si>
-  <si>
-    <t>2 | 20 | 21</t>
-  </si>
-  <si>
-    <t>30 | 19</t>
   </si>
 </sst>
 </file>
@@ -288,7 +288,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -304,7 +304,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,19 +620,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6CF99-69E1-4DA6-A725-47BF4576CF35}">
-  <dimension ref="A1:AK47"/>
+  <dimension ref="A1:AK53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="33" width="18.77734375" customWidth="1"/>
-    <col min="34" max="50" width="15.77734375" customWidth="1"/>
+    <col min="2" max="33" width="18.81640625" customWidth="1"/>
+    <col min="34" max="50" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="4" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" s="4" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -745,7 +745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45515</v>
       </c>
@@ -780,17 +780,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45516</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45517</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45518</v>
       </c>
@@ -825,12 +825,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45519</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45520</v>
       </c>
@@ -868,47 +868,47 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45521</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45522</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45523</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45524</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45525</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45526</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45527</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45528</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45529</v>
       </c>
@@ -946,32 +946,32 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45530</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45531</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45532</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45533</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45534</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45535</v>
       </c>
@@ -1024,37 +1024,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45537</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45538</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45539</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45540</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45541</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45542</v>
       </c>
@@ -1107,42 +1107,42 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45543</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45544</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45545</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45546</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45547</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>45548</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>45549</v>
       </c>
     </row>
-    <row r="37" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>45550</v>
       </c>
@@ -1159,10 +1159,10 @@
         <v>24</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R37" s="3">
         <v>30</v>
@@ -1171,16 +1171,16 @@
         <v>25</v>
       </c>
       <c r="V37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W37" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="W37" s="3" t="s">
+      <c r="Z37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA37" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="Z37" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA37" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="AH37" s="3">
         <v>20</v>
@@ -1189,54 +1189,84 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>45551</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>45552</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>45553</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>45554</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>45555</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>45556</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>45557</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>45558</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45559</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45560</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>45561</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>45562</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>45563</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>45565</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>45566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added page for only one answer generation
</commit_message>
<xml_diff>
--- a/data/davie trainingsplan 2014.xlsx
+++ b/data/davie trainingsplan 2014.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvolf\python_projects\devie_trainer\davie_trainer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\davie_trainer\davie_trainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A756D4-7DBC-4EDA-9676-2AAC8EE1096F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DDA42F-F966-459E-88B3-9CE44490DC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-10365" windowWidth="38640" windowHeight="21120" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>Planke set 1</t>
   </si>
@@ -212,6 +212,9 @@
     <t>30 | 20</t>
   </si>
   <si>
+    <t>2 | 21</t>
+  </si>
+  <si>
     <t>30 | 17</t>
   </si>
   <si>
@@ -227,7 +230,16 @@
     <t>30 | 19</t>
   </si>
   <si>
-    <t>2 | 21</t>
+    <t>2 | 20 | 20</t>
+  </si>
+  <si>
+    <t>2 | 19</t>
+  </si>
+  <si>
+    <t>2 | 20 | 17</t>
+  </si>
+  <si>
+    <t>30 | 22</t>
   </si>
 </sst>
 </file>
@@ -288,7 +300,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -304,7 +316,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,19 +632,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6CF99-69E1-4DA6-A725-47BF4576CF35}">
-  <dimension ref="A1:AK53"/>
+  <dimension ref="A1:AK60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="J38" workbookViewId="0">
+      <selection activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="33" width="18.81640625" customWidth="1"/>
-    <col min="34" max="50" width="15.81640625" customWidth="1"/>
+    <col min="2" max="33" width="18.77734375" customWidth="1"/>
+    <col min="34" max="50" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="4" customFormat="1" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="4" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -745,7 +757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45515</v>
       </c>
@@ -780,17 +792,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45516</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45517</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45518</v>
       </c>
@@ -825,12 +837,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45519</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45520</v>
       </c>
@@ -868,47 +880,47 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45521</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45522</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45523</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45524</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45525</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45526</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45527</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45528</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45529</v>
       </c>
@@ -946,32 +958,32 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45530</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45531</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45532</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45533</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45534</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45535</v>
       </c>
@@ -1024,37 +1036,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45536</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45537</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45538</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45539</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45540</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45541</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45542</v>
       </c>
@@ -1107,166 +1119,243 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45543</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45544</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45545</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45546</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45547</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45548</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45549</v>
       </c>
     </row>
-    <row r="37" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>45550</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37">
         <v>100</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37">
         <v>100</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37">
         <v>24</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37">
         <v>24</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J37" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37" t="s">
+        <v>60</v>
+      </c>
+      <c r="R37">
+        <v>30</v>
+      </c>
+      <c r="S37">
+        <v>25</v>
+      </c>
+      <c r="V37" t="s">
+        <v>61</v>
+      </c>
+      <c r="W37" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA37" t="s">
         <v>63</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R37" s="3">
-        <v>30</v>
-      </c>
-      <c r="S37" s="3">
-        <v>25</v>
-      </c>
-      <c r="V37" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="W37" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z37" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH37" s="3">
+      <c r="AH37">
         <v>20</v>
       </c>
-      <c r="AI37" s="3">
+      <c r="AI37">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45551</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45552</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45553</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45554</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45555</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45556</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45557</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45558</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45559</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45560</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>45561</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>45562</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>45563</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>45564</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>45565</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>45566</v>
+      </c>
+    </row>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>45567</v>
+      </c>
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>45568</v>
+      </c>
+    </row>
+    <row r="56" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B56" s="3">
+        <v>105</v>
+      </c>
+      <c r="C56" s="3">
+        <v>100</v>
+      </c>
+      <c r="F56" s="3">
+        <v>20</v>
+      </c>
+      <c r="G56" s="3">
+        <v>17</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R56" s="3">
+        <v>30</v>
+      </c>
+      <c r="S56" s="3">
+        <v>29</v>
+      </c>
+      <c r="V56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH56" s="3">
+        <v>30</v>
+      </c>
+      <c r="AI56" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>45570</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>45571</v>
+      </c>
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>45572</v>
+      </c>
+    </row>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>45573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added y lims and new data
</commit_message>
<xml_diff>
--- a/data/davie trainingsplan 2014.xlsx
+++ b/data/davie trainingsplan 2014.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\davie_trainer\davie_trainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DDA42F-F966-459E-88B3-9CE44490DC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C180491-F46F-4F5A-A1D4-C70AD46CFF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>Planke set 1</t>
   </si>
@@ -240,6 +240,18 @@
   </si>
   <si>
     <t>30 | 22</t>
+  </si>
+  <si>
+    <t>2 | 20</t>
+  </si>
+  <si>
+    <t>2 | 20 | 18</t>
+  </si>
+  <si>
+    <t>30 | 18</t>
+  </si>
+  <si>
+    <t>2 | 16</t>
   </si>
 </sst>
 </file>
@@ -290,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -298,6 +310,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -632,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6CF99-69E1-4DA6-A725-47BF4576CF35}">
-  <dimension ref="A1:AK60"/>
+  <dimension ref="A1:AK70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J38" workbookViewId="0">
-      <selection activeCell="N58" sqref="N58"/>
+    <sheetView tabSelected="1" topLeftCell="F50" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1291,50 +1305,50 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="56" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
+    <row r="56" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
         <v>45569</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="6">
         <v>105</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="6">
         <v>100</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56" s="6">
         <v>20</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="6">
         <v>17</v>
       </c>
-      <c r="J56" s="3" t="s">
+      <c r="J56" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K56" s="3" t="s">
+      <c r="K56" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="R56" s="3">
+      <c r="R56" s="6">
         <v>30</v>
       </c>
-      <c r="S56" s="3">
+      <c r="S56" s="6">
         <v>29</v>
       </c>
-      <c r="V56" s="3" t="s">
+      <c r="V56" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="W56" s="3" t="s">
+      <c r="W56" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Z56" t="s">
+      <c r="Z56" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AA56" t="s">
+      <c r="AA56" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="AH56" s="3">
+      <c r="AH56" s="6">
         <v>30</v>
       </c>
-      <c r="AI56" s="3">
+      <c r="AI56" s="6">
         <v>25</v>
       </c>
     </row>
@@ -1356,6 +1370,101 @@
     <row r="60" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>45573</v>
+      </c>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>45577</v>
+      </c>
+    </row>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>45580</v>
+      </c>
+    </row>
+    <row r="68" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>45581</v>
+      </c>
+      <c r="B68" s="3">
+        <v>110</v>
+      </c>
+      <c r="C68" s="3">
+        <v>110</v>
+      </c>
+      <c r="F68" s="3">
+        <v>16</v>
+      </c>
+      <c r="G68" s="3">
+        <v>18</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R68" s="3">
+        <v>32</v>
+      </c>
+      <c r="S68" s="3">
+        <v>19</v>
+      </c>
+      <c r="V68" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="W68" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z68" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA68" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH68" s="3">
+        <v>30</v>
+      </c>
+      <c r="AI68" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>45583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new training data
</commit_message>
<xml_diff>
--- a/data/davie trainingsplan 2014.xlsx
+++ b/data/davie trainingsplan 2014.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\davie_trainer\davie_trainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49A6854B-CDF4-4C89-83B1-341696A32D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A648ED5-4B21-4581-B89D-1868C6E221B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-12615" windowWidth="38640" windowHeight="21120" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F844EAE-C179-4864-ABE1-B44B077D5CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Planke set 1</t>
   </si>
@@ -264,6 +264,24 @@
   </si>
   <si>
     <t>2 | 20 | 26</t>
+  </si>
+  <si>
+    <t>2 | 23</t>
+  </si>
+  <si>
+    <t>2 | 20 | 24</t>
+  </si>
+  <si>
+    <t>30 | 26</t>
+  </si>
+  <si>
+    <t>2 | 24</t>
+  </si>
+  <si>
+    <t>1,5 | 20 | 27</t>
+  </si>
+  <si>
+    <t>1,5 | 20 | 24</t>
   </si>
 </sst>
 </file>
@@ -656,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6CF99-69E1-4DA6-A725-47BF4576CF35}">
-  <dimension ref="A1:AK76"/>
+  <dimension ref="A1:AK77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U26" workbookViewId="0">
-      <selection activeCell="AI61" sqref="AI61"/>
+    <sheetView tabSelected="1" topLeftCell="R71" workbookViewId="0">
+      <selection activeCell="V82" sqref="V82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,20 +1498,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
         <v>45584</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71">
         <v>115</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71">
         <v>85</v>
       </c>
-      <c r="F71" s="3">
+      <c r="F71">
         <v>20</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G71">
         <v>21</v>
       </c>
       <c r="J71" t="s">
@@ -1502,10 +1520,10 @@
       <c r="K71" t="s">
         <v>65</v>
       </c>
-      <c r="R71" s="3">
+      <c r="R71">
         <v>32</v>
       </c>
-      <c r="S71" s="3">
+      <c r="S71">
         <v>36</v>
       </c>
       <c r="V71" t="s">
@@ -1547,6 +1565,59 @@
     <row r="76" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>45589</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>45590</v>
+      </c>
+      <c r="B77" s="3">
+        <v>120</v>
+      </c>
+      <c r="C77" s="3">
+        <v>115</v>
+      </c>
+      <c r="F77" s="3">
+        <v>23</v>
+      </c>
+      <c r="G77" s="3">
+        <v>22</v>
+      </c>
+      <c r="H77" s="3">
+        <v>18</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R77" s="3">
+        <v>35</v>
+      </c>
+      <c r="S77" s="3">
+        <v>38</v>
+      </c>
+      <c r="V77" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="W77" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="X77" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z77" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA77" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH77" s="3">
+        <v>40</v>
+      </c>
+      <c r="AI77" s="3">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>